<commit_message>
Refactored code in whiteboard.py
</commit_message>
<xml_diff>
--- a/whiteboards/userdata/users.xlsx
+++ b/whiteboards/userdata/users.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,7 +56,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -68,44 +79,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -132,14 +143,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -166,6 +178,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -177,200 +190,152 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>